<commit_message>
deletion of students working and checks for duplicate entrys
</commit_message>
<xml_diff>
--- a/admin/lists/full_student_list.xlsx
+++ b/admin/lists/full_student_list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Vorname</t>
   </si>
@@ -30,6 +30,36 @@
   </si>
   <si>
     <t>Thema</t>
+  </si>
+  <si>
+    <t>Nina</t>
+  </si>
+  <si>
+    <t>Röckelein</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Berichte schreiben, Vorgangsbeschreibungen</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Mustermann</t>
+  </si>
+  <si>
+    <t>ökjkja</t>
+  </si>
+  <si>
+    <t>yölsvösdm</t>
+  </si>
+  <si>
+    <t>Tempus erkennen (Plusquamperfekt, Perfekt, Präteritum, Präsens, Futur)</t>
+  </si>
+  <si>
+    <t>Mia</t>
   </si>
 </sst>
 </file>
@@ -368,7 +398,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,6 +421,516 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>